<commit_message>
Updates (results from several experiments)
Also, several scripts had minor updates.
</commit_message>
<xml_diff>
--- a/Code/R/Magnan/PerfSearch_Regression_PSF10.xlsx
+++ b/Code/R/Magnan/PerfSearch_Regression_PSF10.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TenfoldCV_Coarse" sheetId="6" r:id="rId1"/>
@@ -841,23 +841,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="39715584"/>
-        <c:axId val="40569088"/>
+        <c:axId val="99453568"/>
+        <c:axId val="99468032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="39715584"/>
+        <c:axId val="99453568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40569088"/>
+        <c:crossAx val="99468032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="40569088"/>
+        <c:axId val="99468032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -865,7 +865,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39715584"/>
+        <c:crossAx val="99453568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -878,7 +878,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2024,23 +2024,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="116761344"/>
-        <c:axId val="116763648"/>
+        <c:axId val="42132608"/>
+        <c:axId val="42134144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="116761344"/>
+        <c:axId val="42132608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116763648"/>
+        <c:crossAx val="42134144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="116763648"/>
+        <c:axId val="42134144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2048,7 +2048,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116761344"/>
+        <c:crossAx val="42132608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2061,7 +2061,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4599,23 +4599,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="39289600"/>
-        <c:axId val="39255040"/>
+        <c:axId val="82027264"/>
+        <c:axId val="82028800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="39289600"/>
+        <c:axId val="82027264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39255040"/>
+        <c:crossAx val="82028800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="39255040"/>
+        <c:axId val="82028800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4623,7 +4623,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39289600"/>
+        <c:crossAx val="82027264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4636,7 +4636,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5035,7 +5035,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5240,9 +5240,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:J247"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E110" sqref="E110"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -12434,7 +12432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B53" sqref="B53"/>
     </sheetView>

</xml_diff>